<commit_message>
Nouveau bon de commande, rempalcement faugeres
</commit_message>
<xml_diff>
--- a/web/download/BonDeCommande.xlsx
+++ b/web/download/BonDeCommande.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Bon de Commande" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Bon de Commande'!$A$2:$I$63</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Bon de Commande'!$A$2:$I$65</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>Bon de Commande</t>
   </si>
@@ -252,6 +252,15 @@
   <si>
     <t>Action valable jusqu'au 17 mai 2016</t>
   </si>
+  <si>
+    <t>Epuisé</t>
+  </si>
+  <si>
+    <t>Château Viranel - Saint-Chinian</t>
+  </si>
+  <si>
+    <t>M1910/13</t>
+  </si>
 </sst>
 </file>
 
@@ -262,7 +271,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.0\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -345,6 +354,13 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.34998626667073579"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -397,7 +413,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -467,9 +483,26 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -900,10 +933,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView showGridLines="0" showRowColHeaders="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:H15"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -922,18 +955,18 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="35" t="s">
+      <c r="D2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="35"/>
-      <c r="F2" s="35"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="E3" s="29"/>
-      <c r="F3" s="29"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" s="26"/>
@@ -943,41 +976,41 @@
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
-      <c r="C5" s="36" t="s">
+      <c r="C5" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="36"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="36"/>
+      <c r="D5" s="44"/>
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25"/>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
+      <c r="G7" s="39"/>
+      <c r="H7" s="39"/>
     </row>
     <row r="8" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="30"/>
-      <c r="H9" s="30"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
     </row>
     <row r="10" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="3"/>
@@ -991,12 +1024,12 @@
       <c r="B11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="30"/>
-      <c r="G11" s="30"/>
-      <c r="H11" s="30"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
     </row>
     <row r="12" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="3"/>
@@ -1011,14 +1044,14 @@
       <c r="B13" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="30"/>
-      <c r="D13" s="30"/>
-      <c r="E13" s="30"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G13" s="30"/>
-      <c r="H13" s="30"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
     </row>
     <row r="14" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
@@ -1030,12 +1063,12 @@
       <c r="B15" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="30"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
     </row>
     <row r="16" spans="1:9" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
@@ -1050,12 +1083,12 @@
       <c r="B17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="30"/>
-      <c r="E17" s="30"/>
-      <c r="F17" s="30"/>
-      <c r="G17" s="30"/>
-      <c r="H17" s="30"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="38"/>
     </row>
     <row r="18" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
@@ -1067,53 +1100,54 @@
       <c r="B19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="38"/>
     </row>
     <row r="20" spans="2:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="3"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45"/>
+      <c r="E21" s="45"/>
+      <c r="F21" s="45"/>
+      <c r="G21" s="45"/>
+      <c r="H21" s="45"/>
     </row>
     <row r="22" spans="2:8" ht="9.9499999999999993" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="31" t="s">
+      <c r="B23" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="31"/>
-      <c r="F23" s="31"/>
-      <c r="G23" s="31"/>
-      <c r="H23" s="31"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
+      <c r="G23" s="39"/>
+      <c r="H23" s="39"/>
     </row>
     <row r="24" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="38" t="s">
+      <c r="C25" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
+      <c r="D25" s="46"/>
+      <c r="E25" s="46"/>
       <c r="F25" s="16" t="s">
         <v>10</v>
       </c>
@@ -1143,7 +1177,9 @@
       <c r="F27" s="8">
         <v>7</v>
       </c>
-      <c r="G27" s="23"/>
+      <c r="G27" s="23">
+        <v>0</v>
+      </c>
       <c r="H27" s="6">
         <f>F27*G27</f>
         <v>0</v>
@@ -1164,9 +1200,11 @@
       <c r="F29" s="8">
         <v>8.5</v>
       </c>
-      <c r="G29" s="23"/>
+      <c r="G29" s="23">
+        <v>0</v>
+      </c>
       <c r="H29" s="6">
-        <f t="shared" ref="H29:H37" si="0">F29*G29</f>
+        <f t="shared" ref="H29:H39" si="0">F29*G29</f>
         <v>0</v>
       </c>
     </row>
@@ -1185,7 +1223,9 @@
       <c r="F31" s="8">
         <v>7.5</v>
       </c>
-      <c r="G31" s="23"/>
+      <c r="G31" s="23">
+        <v>0</v>
+      </c>
       <c r="H31" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1206,7 +1246,9 @@
       <c r="F33" s="8">
         <v>6.5</v>
       </c>
-      <c r="G33" s="23"/>
+      <c r="G33" s="23">
+        <v>0</v>
+      </c>
       <c r="H33" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1227,7 +1269,9 @@
       <c r="F35" s="8">
         <v>11</v>
       </c>
-      <c r="G35" s="23"/>
+      <c r="G35" s="23">
+        <v>0</v>
+      </c>
       <c r="H35" s="6">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -1239,79 +1283,85 @@
       <c r="H36" s="6"/>
     </row>
     <row r="37" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C37" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="F37" s="9">
+      <c r="D37" s="29"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="30">
         <v>12</v>
       </c>
-      <c r="G37" s="24"/>
-      <c r="H37" s="7">
+      <c r="G37" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F38" s="27"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="28"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F39" s="9">
+        <v>12</v>
+      </c>
+      <c r="G39" s="24">
+        <v>0</v>
+      </c>
+      <c r="H39" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="F38" s="10" t="s">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="F40" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="G38" s="11">
-        <f>SUM(G27:G37)</f>
+      <c r="G40" s="11">
+        <f>SUM(G27,G29,G31,G33,G35,G39)</f>
         <v>0</v>
       </c>
-      <c r="H38" s="12">
-        <f>SUM(H27:H37)</f>
+      <c r="H40" s="12">
+        <f>SUM(H27,H29,H31,H33,H35,H39)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B40" s="31" t="s">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B42" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="31"/>
-      <c r="G40" s="31"/>
-      <c r="H40" s="31"/>
-    </row>
-    <row r="41" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="28"/>
-      <c r="F42" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="G42" s="28"/>
-      <c r="H42" s="28"/>
-    </row>
-    <row r="43" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="13"/>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="13"/>
-    </row>
+      <c r="C42" s="39"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="39"/>
+      <c r="H42" s="39"/>
+    </row>
+    <row r="43" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B44" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="28"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="28"/>
-      <c r="H44" s="28"/>
+        <v>1</v>
+      </c>
+      <c r="C44" s="36"/>
+      <c r="D44" s="36"/>
+      <c r="E44" s="36"/>
+      <c r="F44" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="36"/>
+      <c r="H44" s="36"/>
     </row>
     <row r="45" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="13"/>
@@ -1324,14 +1374,14 @@
     </row>
     <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B46" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="28"/>
-      <c r="H46" s="28"/>
+        <v>25</v>
+      </c>
+      <c r="C46" s="13"/>
+      <c r="D46" s="36"/>
+      <c r="E46" s="36"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="36"/>
     </row>
     <row r="47" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="13"/>
@@ -1344,181 +1394,201 @@
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" s="28"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="28"/>
-      <c r="F48" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
+        <v>7</v>
+      </c>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
     </row>
     <row r="49" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B49" s="13"/>
+      <c r="C49" s="13"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+      <c r="G49" s="13"/>
+      <c r="H49" s="13"/>
     </row>
     <row r="50" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B50" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="C50" s="30"/>
-      <c r="D50" s="30"/>
-      <c r="E50" s="30"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="30"/>
-      <c r="H50" s="30"/>
+        <v>3</v>
+      </c>
+      <c r="C50" s="36"/>
+      <c r="D50" s="36"/>
+      <c r="E50" s="36"/>
+      <c r="F50" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="36"/>
+      <c r="H50" s="36"/>
     </row>
     <row r="51" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="13"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B52" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C52" s="38"/>
+      <c r="D52" s="38"/>
+      <c r="E52" s="38"/>
+      <c r="F52" s="38"/>
+      <c r="G52" s="38"/>
+      <c r="H52" s="38"/>
+    </row>
+    <row r="53" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="13"/>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B54" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C52" s="30"/>
-      <c r="D52" s="30"/>
-      <c r="E52" s="30"/>
-      <c r="F52" s="30"/>
-      <c r="G52" s="30"/>
-      <c r="H52" s="30"/>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" s="33" t="s">
+      <c r="C54" s="38"/>
+      <c r="D54" s="38"/>
+      <c r="E54" s="38"/>
+      <c r="F54" s="38"/>
+      <c r="G54" s="38"/>
+      <c r="H54" s="38"/>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B56" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="C54" s="33"/>
-      <c r="D54" s="33"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-    </row>
-    <row r="55" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="22"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="22"/>
-      <c r="E55" s="22"/>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="22"/>
-    </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B56" s="34" t="s">
+      <c r="C56" s="41"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="41"/>
+      <c r="H56" s="41"/>
+    </row>
+    <row r="57" spans="2:8" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="22"/>
+      <c r="C57" s="22"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="22"/>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="22"/>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B58" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="C56" s="33"/>
-      <c r="D56" s="33"/>
-      <c r="E56" s="33"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="33"/>
-      <c r="H56" s="33"/>
-    </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B57" s="33" t="s">
+      <c r="C58" s="41"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
+      <c r="F58" s="41"/>
+      <c r="G58" s="41"/>
+      <c r="H58" s="41"/>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B59" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="33"/>
-      <c r="D57" s="33"/>
-      <c r="E57" s="33"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="33"/>
-      <c r="H57" s="33"/>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" s="33" t="s">
+      <c r="C59" s="41"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
+      <c r="F59" s="41"/>
+      <c r="G59" s="41"/>
+      <c r="H59" s="41"/>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B60" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C58" s="33"/>
-      <c r="D58" s="33"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-    </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B59" s="33" t="s">
+      <c r="C60" s="41"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
+      <c r="F60" s="41"/>
+      <c r="G60" s="41"/>
+      <c r="H60" s="41"/>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B61" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C59" s="33"/>
-      <c r="D59" s="33"/>
-      <c r="E59" s="33"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="33"/>
-      <c r="H59" s="33"/>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" s="33" t="s">
+      <c r="C61" s="41"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
+      <c r="F61" s="41"/>
+      <c r="G61" s="41"/>
+      <c r="H61" s="41"/>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B62" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="33"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="33"/>
-      <c r="H60" s="33"/>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B61" s="33" t="s">
+      <c r="C62" s="41"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
+      <c r="F62" s="41"/>
+      <c r="G62" s="41"/>
+      <c r="H62" s="41"/>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B63" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C61" s="33"/>
-      <c r="D61" s="33"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="33"/>
-      <c r="G61" s="33"/>
-      <c r="H61" s="33"/>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B62" s="32"/>
-      <c r="C62" s="32"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
-    </row>
-    <row r="63" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
-      <c r="B63" s="32"/>
-      <c r="C63" s="32"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="32"/>
-    </row>
-    <row r="64" spans="2:8" hidden="1" x14ac:dyDescent="0.25"/>
-    <row r="65" hidden="1" x14ac:dyDescent="0.25"/>
+      <c r="C63" s="41"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="41"/>
+      <c r="F63" s="41"/>
+      <c r="G63" s="41"/>
+      <c r="H63" s="41"/>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B64" s="40"/>
+      <c r="C64" s="40"/>
+      <c r="D64" s="40"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="40"/>
+      <c r="H64" s="40"/>
+    </row>
+    <row r="65" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="40"/>
+      <c r="C65" s="40"/>
+      <c r="D65" s="40"/>
+      <c r="E65" s="40"/>
+      <c r="F65" s="40"/>
+      <c r="G65" s="40"/>
+      <c r="H65" s="40"/>
+    </row>
+    <row r="66" spans="2:8" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:8" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection password="B43D" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="33">
     <mergeCell ref="D2:F2"/>
     <mergeCell ref="C5:G5"/>
     <mergeCell ref="B21:H21"/>
-    <mergeCell ref="B60:H60"/>
-    <mergeCell ref="B61:H61"/>
-    <mergeCell ref="C50:H50"/>
+    <mergeCell ref="B62:H62"/>
+    <mergeCell ref="B63:H63"/>
     <mergeCell ref="C52:H52"/>
-    <mergeCell ref="G48:H48"/>
+    <mergeCell ref="C54:H54"/>
+    <mergeCell ref="G50:H50"/>
     <mergeCell ref="C15:H15"/>
     <mergeCell ref="D19:H19"/>
     <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B40:H40"/>
-    <mergeCell ref="C42:E42"/>
-    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="G44:H44"/>
     <mergeCell ref="B23:H23"/>
     <mergeCell ref="C17:H17"/>
-    <mergeCell ref="B62:H62"/>
-    <mergeCell ref="B63:H63"/>
-    <mergeCell ref="B54:H54"/>
+    <mergeCell ref="B64:H64"/>
+    <mergeCell ref="B65:H65"/>
     <mergeCell ref="B56:H56"/>
-    <mergeCell ref="B57:H57"/>
     <mergeCell ref="B58:H58"/>
     <mergeCell ref="B59:H59"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C46:H46"/>
-    <mergeCell ref="D44:H44"/>
+    <mergeCell ref="B60:H60"/>
+    <mergeCell ref="B61:H61"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C48:H48"/>
+    <mergeCell ref="D46:H46"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="C11:H11"/>
     <mergeCell ref="C9:E9"/>

</xml_diff>